<commit_message>
updated instructions and removed dependancies on unused modules
</commit_message>
<xml_diff>
--- a/test folder (02190A)/ASSY Config.xlsx
+++ b/test folder (02190A)/ASSY Config.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="143">
   <si>
     <t>Encoding:</t>
   </si>
@@ -76,7 +76,7 @@
     <t>Creation Date:</t>
   </si>
   <si>
-    <t>24/03/2021</t>
+    <t>25/03/2021</t>
   </si>
   <si>
     <t>Designator</t>
@@ -133,6 +133,9 @@
     <t>Keystone Electronics</t>
   </si>
   <si>
+    <t>1043</t>
+  </si>
+  <si>
     <t>Digi-Key</t>
   </si>
   <si>
@@ -202,13 +205,13 @@
     <t>Header 2x1 RA TH</t>
   </si>
   <si>
-    <t>TSW-102-08-G-S-RA</t>
+    <t>TSW-102-08-L-S-RA</t>
   </si>
   <si>
     <t>SAM1043-02-ND</t>
   </si>
   <si>
-    <t>TSW-102-08-L-S-RA</t>
+    <t>TSW-102-08-F-S-RA</t>
   </si>
   <si>
     <t>SAM10325-ND</t>
@@ -223,9 +226,21 @@
     <t>Jumper 0805 2 pos</t>
   </si>
   <si>
+    <t>Panasonic</t>
+  </si>
+  <si>
+    <t>ERJ-6GEY0R00V</t>
+  </si>
+  <si>
     <t>P0.0ACT-ND</t>
   </si>
   <si>
+    <t>Yageo</t>
+  </si>
+  <si>
+    <t>RC0805FR-070RL</t>
+  </si>
+  <si>
     <t>311-0.0CRCT-ND</t>
   </si>
   <si>
@@ -235,9 +250,18 @@
     <t>Resistor 0R 2512 1W</t>
   </si>
   <si>
+    <t>RC2512JK-070RL</t>
+  </si>
+  <si>
     <t>YAG1232CT-ND</t>
   </si>
   <si>
+    <t>Stackpole Electronics</t>
+  </si>
+  <si>
+    <t>RMCF2512ZT0R00</t>
+  </si>
+  <si>
     <t>RMCF2512ZT0R00CT-ND</t>
   </si>
   <si>
@@ -250,7 +274,13 @@
     <t>Testpoint Hook</t>
   </si>
   <si>
+    <t>5016</t>
+  </si>
+  <si>
     <t>36-5016CT-ND</t>
+  </si>
+  <si>
+    <t>5018</t>
   </si>
   <si>
     <t>36-5018CT-ND</t>
@@ -2352,7 +2382,7 @@
         <v>17</v>
       </c>
       <c r="G2" s="58" t="n">
-        <v>0</v>
+        <v>18.03</v>
       </c>
       <c r="H2" s="18" t="s"/>
       <c r="I2" s="18" t="s"/>
@@ -2475,221 +2505,253 @@
       <c r="F7" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="G7" s="62" t="n">
-        <v>1043</v>
+      <c r="G7" s="62" t="s">
+        <v>38</v>
       </c>
       <c r="H7" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" s="62" t="s">
+        <v>40</v>
+      </c>
+      <c r="J7" s="62" t="s">
+        <v>37</v>
+      </c>
+      <c r="K7" s="62" t="s">
         <v>38</v>
       </c>
-      <c r="I7" s="62" t="s">
-        <v>39</v>
-      </c>
-      <c r="J7" s="62" t="s"/>
-      <c r="K7" s="62" t="s"/>
       <c r="L7" s="67" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="M7" s="67" t="s">
-        <v>41</v>
-      </c>
-      <c r="N7" s="68" t="s"/>
+        <v>42</v>
+      </c>
+      <c r="N7" s="68" t="n">
+        <v>10.32</v>
+      </c>
     </row>
     <row customFormat="1" customHeight="1" ht="16.5" r="8" s="32" spans="1:14">
       <c r="A8" s="62" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B8" s="63" t="s"/>
       <c r="C8" s="64" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D8" s="65" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E8" s="66" t="n">
         <v>2</v>
       </c>
       <c r="F8" s="64" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G8" s="64" t="s">
+        <v>47</v>
+      </c>
+      <c r="H8" s="64" t="s">
+        <v>39</v>
+      </c>
+      <c r="I8" s="64" t="s">
+        <v>48</v>
+      </c>
+      <c r="J8" s="64" t="s">
         <v>46</v>
       </c>
-      <c r="H8" s="64" t="s">
-        <v>38</v>
-      </c>
-      <c r="I8" s="64" t="s">
-        <v>47</v>
-      </c>
-      <c r="J8" s="64" t="s">
-        <v>45</v>
-      </c>
       <c r="K8" s="64" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="L8" s="67" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M8" s="67" t="s">
-        <v>49</v>
-      </c>
-      <c r="N8" s="68" t="s"/>
+        <v>50</v>
+      </c>
+      <c r="N8" s="68" t="n">
+        <v>2.16</v>
+      </c>
     </row>
     <row customFormat="1" customHeight="1" ht="16.5" r="9" s="32" spans="1:14">
       <c r="A9" s="62" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B9" s="63" t="s"/>
       <c r="C9" s="64" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D9" s="65" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E9" s="66" t="n">
         <v>1</v>
       </c>
       <c r="F9" s="62" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G9" s="62" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H9" s="62" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I9" s="62" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J9" s="62" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K9" s="62" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L9" s="67" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M9" s="67" t="s">
-        <v>56</v>
-      </c>
-      <c r="N9" s="68" t="s"/>
+        <v>57</v>
+      </c>
+      <c r="N9" s="68" t="n">
+        <v>0.95</v>
+      </c>
     </row>
     <row customFormat="1" customHeight="1" ht="16.5" r="10" s="32" spans="1:14">
       <c r="A10" s="62" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B10" s="63" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C10" s="64" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D10" s="65" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E10" s="66" t="n">
         <v>2</v>
       </c>
       <c r="F10" s="64" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G10" s="64" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H10" s="64" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I10" s="64" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="J10" s="64" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K10" s="64" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="L10" s="67" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M10" s="67" t="s">
-        <v>64</v>
-      </c>
-      <c r="N10" s="68" t="s"/>
+        <v>65</v>
+      </c>
+      <c r="N10" s="68" t="n">
+        <v>0.75</v>
+      </c>
     </row>
     <row customFormat="1" customHeight="1" ht="16.5" r="11" s="32" spans="1:14">
       <c r="A11" s="62" t="s"/>
       <c r="B11" s="63" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C11" s="64" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D11" s="65" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E11" s="66" t="n">
         <v>0</v>
       </c>
-      <c r="F11" s="62" t="s"/>
-      <c r="G11" s="62" t="s"/>
+      <c r="F11" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11" s="62" t="s">
+        <v>70</v>
+      </c>
       <c r="H11" s="62" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I11" s="62" t="s">
-        <v>68</v>
-      </c>
-      <c r="J11" s="62" t="s"/>
-      <c r="K11" s="62" t="s"/>
+        <v>71</v>
+      </c>
+      <c r="J11" s="62" t="s">
+        <v>72</v>
+      </c>
+      <c r="K11" s="62" t="s">
+        <v>73</v>
+      </c>
       <c r="L11" s="67" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M11" s="67" t="s">
-        <v>69</v>
-      </c>
-      <c r="N11" s="68" t="s"/>
+        <v>74</v>
+      </c>
+      <c r="N11" s="68" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row customFormat="1" customHeight="1" ht="16.5" r="12" s="32" spans="1:14">
       <c r="A12" s="62" t="s"/>
       <c r="B12" s="63" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C12" s="64" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D12" s="65" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="E12" s="66" t="n">
         <v>0</v>
       </c>
-      <c r="F12" s="64" t="s"/>
-      <c r="G12" s="64" t="s"/>
+      <c r="F12" s="64" t="s">
+        <v>72</v>
+      </c>
+      <c r="G12" s="64" t="s">
+        <v>77</v>
+      </c>
       <c r="H12" s="64" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I12" s="64" t="s">
-        <v>72</v>
-      </c>
-      <c r="J12" s="64" t="s"/>
-      <c r="K12" s="64" t="s"/>
+        <v>78</v>
+      </c>
+      <c r="J12" s="64" t="s">
+        <v>79</v>
+      </c>
+      <c r="K12" s="64" t="s">
+        <v>80</v>
+      </c>
       <c r="L12" s="67" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M12" s="67" t="s">
-        <v>73</v>
-      </c>
-      <c r="N12" s="68" t="s"/>
+        <v>81</v>
+      </c>
+      <c r="N12" s="68" t="n">
+        <v>1.55</v>
+      </c>
     </row>
     <row customFormat="1" customHeight="1" ht="16.5" r="13" s="32" spans="1:14">
       <c r="A13" s="62" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="B13" s="63" t="s"/>
       <c r="C13" s="64" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="D13" s="65" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="E13" s="66" t="n">
         <v>5</v>
@@ -2697,28 +2759,30 @@
       <c r="F13" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="G13" s="62" t="n">
-        <v>5018</v>
+      <c r="G13" s="62" t="s">
+        <v>85</v>
       </c>
       <c r="H13" s="62" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I13" s="62" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="J13" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="K13" s="62" t="n">
-        <v>5016</v>
+      <c r="K13" s="62" t="s">
+        <v>87</v>
       </c>
       <c r="L13" s="67" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M13" s="67" t="s">
-        <v>78</v>
-      </c>
-      <c r="N13" s="68" t="s"/>
+        <v>88</v>
+      </c>
+      <c r="N13" s="68" t="n">
+        <v>2.2</v>
+      </c>
     </row>
     <row customFormat="1" customHeight="1" ht="16.5" r="14" s="32" spans="1:14">
       <c r="A14" s="40" t="s"/>
@@ -3814,41 +3878,41 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="E2" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="F2" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="I2" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="J2" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="K2" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="M2" t="s">
         <v>1</v>
       </c>
       <c r="O2" s="53" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="Q2" s="22" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="R2" s="53" t="n"/>
       <c r="T2" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="W2" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="Y2" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="Z2" s="53" t="s">
         <v>3</v>
@@ -3964,7 +4028,7 @@
         <v/>
       </c>
       <c r="Q4" s="54" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="R4" s="53" t="n">
         <v>1</v>
@@ -4024,7 +4088,7 @@
         <v/>
       </c>
       <c r="Q5" s="54" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="R5" s="53" t="n">
         <v>2</v>
@@ -4084,7 +4148,7 @@
         <v/>
       </c>
       <c r="Q6" s="54" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="R6" s="53" t="n">
         <v>3</v>
@@ -4144,7 +4208,7 @@
         <v/>
       </c>
       <c r="Q7" s="54" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="R7" s="53" t="n">
         <v>4</v>
@@ -4192,7 +4256,7 @@
         <v/>
       </c>
       <c r="Q8" s="54" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="R8" s="53" t="n">
         <v>5</v>
@@ -4236,7 +4300,7 @@
         <v>6</v>
       </c>
       <c r="Q9" s="54" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="R9" s="53" t="n">
         <v>6</v>
@@ -4274,10 +4338,10 @@
         <v>7</v>
       </c>
       <c r="I10" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="Q10" s="54" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="R10" s="53" t="n">
         <v>7</v>
@@ -4317,7 +4381,7 @@
         <v/>
       </c>
       <c r="Q11" s="54" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="R11" s="53" t="n">
         <v>8</v>
@@ -4353,7 +4417,7 @@
         <v>9</v>
       </c>
       <c r="Q12" s="54" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="R12" s="53" t="n">
         <v>9</v>
@@ -4386,10 +4450,10 @@
         <v>10</v>
       </c>
       <c r="G13" s="53" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="Q13" s="53" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="R13" s="53" t="n">
         <v>10</v>
@@ -4422,10 +4486,10 @@
         <v>11</v>
       </c>
       <c r="G14" s="53" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="Q14" s="53" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="R14" s="53" t="n">
         <v>11</v>
@@ -4458,10 +4522,10 @@
         <v>12</v>
       </c>
       <c r="G15" s="53" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="Q15" s="53" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="R15" s="53" t="n">
         <v>12</v>
@@ -4494,10 +4558,10 @@
         <v>13</v>
       </c>
       <c r="G16" s="53" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="Q16" s="53" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="R16" s="53" t="n">
         <v>13</v>
@@ -4530,10 +4594,10 @@
         <v>14</v>
       </c>
       <c r="G17" s="53" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="Q17" s="53" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="R17" s="53" t="n">
         <v>14</v>
@@ -4566,10 +4630,10 @@
         <v>15</v>
       </c>
       <c r="G18" s="53" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="Q18" s="53" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="R18" s="53" t="n">
         <v>15</v>
@@ -4602,10 +4666,10 @@
         <v>16</v>
       </c>
       <c r="G19" s="53" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="Q19" s="53" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="R19" s="53" t="n">
         <v>16</v>
@@ -4638,10 +4702,10 @@
         <v>17</v>
       </c>
       <c r="G20" s="53" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="Q20" s="53" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="R20" s="53" t="n">
         <v>17</v>
@@ -4674,10 +4738,10 @@
         <v>18</v>
       </c>
       <c r="G21" s="53" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="Q21" s="53" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="R21" s="53" t="n">
         <v>18</v>
@@ -4710,10 +4774,10 @@
         <v>19</v>
       </c>
       <c r="G22" s="53" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="Q22" s="53" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="R22" s="53" t="n">
         <v>19</v>
@@ -4746,10 +4810,10 @@
         <v>20</v>
       </c>
       <c r="G23" s="53" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="Q23" s="53" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="R23" s="53" t="n">
         <v>20</v>
@@ -4782,10 +4846,10 @@
         <v>21</v>
       </c>
       <c r="G24" s="53" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="Q24" s="53" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="R24" s="53" t="n">
         <v>21</v>
@@ -4818,10 +4882,10 @@
         <v>22</v>
       </c>
       <c r="G25" s="53" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="Q25" s="53" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="R25" s="53" t="n">
         <v>22</v>
@@ -4854,10 +4918,10 @@
         <v>23</v>
       </c>
       <c r="G26" s="53" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="Q26" s="53" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="R26" s="53" t="n">
         <v>23</v>
@@ -4879,10 +4943,10 @@
         <v>24</v>
       </c>
       <c r="G27" s="53" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="Q27" s="53" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="R27" s="53" t="n">
         <v>24</v>
@@ -4893,10 +4957,10 @@
         <v>25</v>
       </c>
       <c r="G28" s="53" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="Q28" s="53" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="R28" s="53" t="n">
         <v>25</v>
@@ -4907,10 +4971,10 @@
         <v>26</v>
       </c>
       <c r="G29" s="53" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="Q29" s="53" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="R29" s="53" t="n">
         <v>26</v>
@@ -4921,10 +4985,10 @@
         <v>27</v>
       </c>
       <c r="G30" s="53" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="Q30" s="53" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="R30" s="53" t="n">
         <v>27</v>
@@ -4935,10 +4999,10 @@
         <v>28</v>
       </c>
       <c r="G31" s="53" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="Q31" s="53" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="R31" s="53" t="n">
         <v>28</v>
@@ -4949,10 +5013,10 @@
         <v>29</v>
       </c>
       <c r="G32" s="53" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="Q32" s="53" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="R32" s="53" t="n">
         <v>29</v>
@@ -5016,13 +5080,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="B1" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="C1" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -5030,10 +5094,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="C2" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -5041,10 +5105,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="C3" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -5052,10 +5116,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="C4" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -5063,10 +5127,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="C5" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -5074,10 +5138,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="C6" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -5085,10 +5149,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="C7" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -5096,10 +5160,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="C8" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -5107,10 +5171,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="C9" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -5118,10 +5182,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="C10" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -5129,10 +5193,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="C11" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -5140,10 +5204,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="C12" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -5151,10 +5215,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="C13" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -5162,10 +5226,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="C14" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -5173,10 +5237,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="C15" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -5184,10 +5248,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="C16" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -5195,10 +5259,10 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="C17" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -5206,10 +5270,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="C18" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -5217,10 +5281,10 @@
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="C19" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -5228,10 +5292,10 @@
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="C20" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -5239,10 +5303,10 @@
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="C21" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -5250,10 +5314,10 @@
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="C22" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -5261,10 +5325,10 @@
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="C23" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -5272,10 +5336,10 @@
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="C24" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -5283,35 +5347,35 @@
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="C25" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="B26" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="B27" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="B28" s="1" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="B29" s="1" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="B30" s="1" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reworked the BOM generation script to accept the new Altium outputs, should result in more reliable BOM generation
</commit_message>
<xml_diff>
--- a/test folder (02190A)/ASSY Config.xlsx
+++ b/test folder (02190A)/ASSY Config.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="138">
   <si>
     <t>Encoding:</t>
   </si>
@@ -76,7 +76,7 @@
     <t>Creation Date:</t>
   </si>
   <si>
-    <t>25/03/2021</t>
+    <t>16/07/2021</t>
   </si>
   <si>
     <t>Designator</t>
@@ -124,7 +124,7 @@
     <t>B1, B2, B3, B4</t>
   </si>
   <si>
-    <t>02190A0: B1, B2, B3, B4</t>
+    <t>705-02190A: B1, B2, B3, B4</t>
   </si>
   <si>
     <t>Battery 18650 Holder</t>
@@ -133,9 +133,6 @@
     <t>Keystone Electronics</t>
   </si>
   <si>
-    <t>1043</t>
-  </si>
-  <si>
     <t>Digi-Key</t>
   </si>
   <si>
@@ -148,58 +145,94 @@
     <t>534-1043</t>
   </si>
   <si>
+    <t>VC0, VC1, VC2, VC3, VC4</t>
+  </si>
+  <si>
+    <t>705-02190A: VC0, VC1, VC2, VC3, VC4</t>
+  </si>
+  <si>
+    <t>Testpoint Hook</t>
+  </si>
+  <si>
+    <t>36-5018CT-ND</t>
+  </si>
+  <si>
+    <t>36-5016CT-ND</t>
+  </si>
+  <si>
+    <t>JP10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">705-02190A: </t>
+  </si>
+  <si>
+    <t>Jumper 0805 2 pos</t>
+  </si>
+  <si>
+    <t>Panasonic</t>
+  </si>
+  <si>
+    <t>ERJ-6GEY0R00V</t>
+  </si>
+  <si>
+    <t>P0.0ACT-ND</t>
+  </si>
+  <si>
+    <t>Yageo</t>
+  </si>
+  <si>
+    <t>RC0805FR-070RL</t>
+  </si>
+  <si>
+    <t>311-0.0CRCT-ND</t>
+  </si>
+  <si>
+    <t>H3</t>
+  </si>
+  <si>
+    <t>705-02190A: H3</t>
+  </si>
+  <si>
+    <t>Header 2x2 TH thru-board 2mm</t>
+  </si>
+  <si>
+    <t>Samtec</t>
+  </si>
+  <si>
+    <t>MTMM-102-02-G-D-196</t>
+  </si>
+  <si>
+    <t>MTMM-102-02-G-D-196-ND</t>
+  </si>
+  <si>
+    <t>MTMM-102-02-S-D-196</t>
+  </si>
+  <si>
     <t>H1, H2</t>
   </si>
   <si>
-    <t>02190A0: H1, H2</t>
+    <t>705-02190A: H1, H2</t>
   </si>
   <si>
     <t>Header 3x2 TH thru-board 2mm</t>
   </si>
   <si>
-    <t>Samtec</t>
+    <t>MTMM-103-03-G-D-000</t>
+  </si>
+  <si>
+    <t>MTMM-103-03-G-D-000-ND</t>
   </si>
   <si>
     <t>MTMM-103-03-G-D-243</t>
   </si>
   <si>
-    <t>MTMM-103-03-G-D-243-ND</t>
-  </si>
-  <si>
-    <t>MTMM-103-03-G-D-000</t>
-  </si>
-  <si>
-    <t>MTMM-103-03-G-D-000-ND</t>
-  </si>
-  <si>
-    <t>H3</t>
-  </si>
-  <si>
-    <t>02190A0: H3</t>
-  </si>
-  <si>
-    <t>Header 2x2 TH thru-board 2mm</t>
-  </si>
-  <si>
-    <t>MTMM-102-02-S-D-196</t>
-  </si>
-  <si>
-    <t>MTMM-102-02-S-D-196-ND</t>
-  </si>
-  <si>
-    <t>MTMM-102-02-G-D-196</t>
-  </si>
-  <si>
-    <t>MTMM-102-02-G-D-196-ND</t>
-  </si>
-  <si>
     <t>JP2, JP4</t>
   </si>
   <si>
     <t>JP3</t>
   </si>
   <si>
-    <t>02190A0: JP2, JP4</t>
+    <t>705-02190A: JP2, JP4</t>
   </si>
   <si>
     <t>Header 2x1 RA TH</t>
@@ -217,73 +250,25 @@
     <t>SAM10325-ND</t>
   </si>
   <si>
-    <t>JP10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">02190A0: </t>
-  </si>
-  <si>
-    <t>Jumper 0805 2 pos</t>
-  </si>
-  <si>
-    <t>Panasonic</t>
-  </si>
-  <si>
-    <t>ERJ-6GEY0R00V</t>
-  </si>
-  <si>
-    <t>P0.0ACT-ND</t>
-  </si>
-  <si>
-    <t>Yageo</t>
-  </si>
-  <si>
-    <t>RC0805FR-070RL</t>
-  </si>
-  <si>
-    <t>311-0.0CRCT-ND</t>
-  </si>
-  <si>
     <t>R52, R53, R65, R73, R76</t>
   </si>
   <si>
     <t>Resistor 0R 2512 1W</t>
   </si>
   <si>
+    <t>Stackpole Electronics</t>
+  </si>
+  <si>
+    <t>RMCF2512ZT0R00</t>
+  </si>
+  <si>
+    <t>RMCF2512ZT0R00CT-ND</t>
+  </si>
+  <si>
     <t>RC2512JK-070RL</t>
   </si>
   <si>
     <t>YAG1232CT-ND</t>
-  </si>
-  <si>
-    <t>Stackpole Electronics</t>
-  </si>
-  <si>
-    <t>RMCF2512ZT0R00</t>
-  </si>
-  <si>
-    <t>RMCF2512ZT0R00CT-ND</t>
-  </si>
-  <si>
-    <t>VC0, VC1, VC2, VC3, VC4</t>
-  </si>
-  <si>
-    <t>02190A0: VC0, VC1, VC2, VC3, VC4</t>
-  </si>
-  <si>
-    <t>Testpoint Hook</t>
-  </si>
-  <si>
-    <t>5016</t>
-  </si>
-  <si>
-    <t>36-5016CT-ND</t>
-  </si>
-  <si>
-    <t>5018</t>
-  </si>
-  <si>
-    <t>36-5018CT-ND</t>
   </si>
   <si>
     <t>bit value</t>
@@ -560,7 +545,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -684,20 +669,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0"/>
     <xf borderId="1" fillId="3" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="63">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
@@ -858,27 +836,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf borderId="8" fillId="0" fontId="10" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="11" fillId="0" fontId="10" numFmtId="0" pivotButton="0" quotePrefix="1" xfId="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="11" fillId="0" fontId="10" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="11" fillId="0" fontId="10" numFmtId="0" pivotButton="0" quotePrefix="1" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="11" fillId="0" fontId="10" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf applyAlignment="1" borderId="11" fillId="0" fontId="10" numFmtId="0" pivotButton="0" quotePrefix="1" xfId="0">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="11" fillId="0" fontId="10" numFmtId="0" pivotButton="0" quotePrefix="1" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf applyAlignment="1" borderId="11" fillId="0" fontId="10" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="10" numFmtId="0" pivotButton="0" quotePrefix="1" xfId="0">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
@@ -1807,7 +1764,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N79"/>
+  <dimension ref="A1:O79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
       <selection activeCell="H5" sqref="H5"/>
@@ -2336,7 +2293,7 @@
     <col customWidth="1" max="16384" min="16143" style="34" width="9.140625"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="37.5" r="1" s="30" spans="1:14">
+    <row customHeight="1" ht="37.5" r="1" s="30" spans="1:15">
       <c r="A1" s="56" t="s">
         <v>7</v>
       </c>
@@ -2363,8 +2320,9 @@
       <c r="L1" s="13" t="s"/>
       <c r="M1" s="13" t="s"/>
       <c r="N1" s="14" t="s"/>
-    </row>
-    <row customHeight="1" ht="23.25" r="2" s="30" spans="1:14">
+      <c r="O1" t="s"/>
+    </row>
+    <row customHeight="1" ht="23.25" r="2" s="30" spans="1:15">
       <c r="A2" s="15" t="s">
         <v>13</v>
       </c>
@@ -2382,7 +2340,7 @@
         <v>17</v>
       </c>
       <c r="G2" s="58" t="n">
-        <v>18.03</v>
+        <v>0</v>
       </c>
       <c r="H2" s="18" t="s"/>
       <c r="I2" s="18" t="s"/>
@@ -2391,8 +2349,9 @@
       <c r="L2" t="s"/>
       <c r="M2" t="s"/>
       <c r="N2" s="19" t="s"/>
-    </row>
-    <row r="3" spans="1:14">
+      <c r="O2" t="s"/>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="20" t="s"/>
       <c r="B3" s="21" t="s"/>
       <c r="C3" s="22" t="s"/>
@@ -2407,8 +2366,9 @@
       <c r="L3" s="23" t="s"/>
       <c r="M3" s="23" t="s"/>
       <c r="N3" s="24" t="s"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="4" s="30" spans="1:14">
+      <c r="O3" t="s"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="4" s="30" spans="1:15">
       <c r="A4" s="61" t="s">
         <v>18</v>
       </c>
@@ -2427,8 +2387,9 @@
       <c r="L4" s="27" t="s"/>
       <c r="M4" s="27" t="s"/>
       <c r="N4" s="28" t="s"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="5" s="30" spans="1:14">
+      <c r="O4" t="s"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="5" s="30" spans="1:15">
       <c r="A5" s="29" t="s"/>
       <c r="B5" s="22" t="s"/>
       <c r="C5" s="22" t="s"/>
@@ -2443,8 +2404,9 @@
       <c r="L5" t="s"/>
       <c r="M5" t="s"/>
       <c r="N5" s="28" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="19.5" r="6" s="31" spans="1:14">
+      <c r="O5" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="19.5" r="6" s="31" spans="1:15">
       <c r="A6" s="35" t="s">
         <v>20</v>
       </c>
@@ -2487,309 +2449,313 @@
       <c r="N6" s="38" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="7" s="32" spans="1:14">
-      <c r="A7" s="62" t="s">
+      <c r="O6" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="7" s="32" spans="1:15">
+      <c r="A7" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="63" t="s"/>
-      <c r="C7" s="64" t="s">
+      <c r="B7" s="41" t="s"/>
+      <c r="C7" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="65" t="s">
+      <c r="D7" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="66" t="n">
+      <c r="E7" s="62" t="n">
         <v>4</v>
       </c>
-      <c r="F7" s="62" t="s">
+      <c r="F7" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="G7" s="62" t="s">
+      <c r="G7" s="40" t="n">
+        <v>1043</v>
+      </c>
+      <c r="H7" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="62" t="s">
+      <c r="I7" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="62" t="s">
+      <c r="J7" s="40" t="s"/>
+      <c r="K7" s="40" t="s"/>
+      <c r="L7" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="J7" s="62" t="s">
+      <c r="M7" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="N7" s="45" t="n">
+        <v>12.56</v>
+      </c>
+      <c r="O7" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="8" s="32" spans="1:15">
+      <c r="A8" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="41" t="s"/>
+      <c r="C8" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="62" t="n">
+        <v>5</v>
+      </c>
+      <c r="F8" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="K7" s="62" t="s">
+      <c r="G8" s="42" t="n">
+        <v>5018</v>
+      </c>
+      <c r="H8" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="L7" s="67" t="s">
-        <v>41</v>
-      </c>
-      <c r="M7" s="67" t="s">
-        <v>42</v>
-      </c>
-      <c r="N7" s="68" t="n">
-        <v>10.32</v>
-      </c>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="8" s="32" spans="1:14">
-      <c r="A8" s="62" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="63" t="s"/>
-      <c r="C8" s="64" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="65" t="s">
+      <c r="I8" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="66" t="n">
+      <c r="J8" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="K8" s="42" t="n">
+        <v>5016</v>
+      </c>
+      <c r="L8" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="M8" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="N8" s="45" t="n">
+        <v>1.95</v>
+      </c>
+      <c r="O8" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="9" s="32" spans="1:15">
+      <c r="A9" s="40" t="s"/>
+      <c r="B9" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="H9" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="I9" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="J9" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="K9" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="L9" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="M9" s="44" t="s">
+        <v>55</v>
+      </c>
+      <c r="N9" s="45" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="10" s="32" spans="1:15">
+      <c r="A10" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="41" t="s"/>
+      <c r="C10" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="62" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="G10" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="H10" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="I10" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="J10" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="K10" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="L10" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="M10" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="N10" s="45" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="O10" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="11" s="32" spans="1:15">
+      <c r="A11" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="41" t="s"/>
+      <c r="C11" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" s="62" t="n">
         <v>2</v>
       </c>
-      <c r="F8" s="64" t="s">
-        <v>46</v>
-      </c>
-      <c r="G8" s="64" t="s">
-        <v>47</v>
-      </c>
-      <c r="H8" s="64" t="s">
-        <v>39</v>
-      </c>
-      <c r="I8" s="64" t="s">
+      <c r="F11" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="H11" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="I11" s="40" t="s">
+        <v>67</v>
+      </c>
+      <c r="J11" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="K11" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="L11" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="M11" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="N11" s="45" t="n">
+        <v>3</v>
+      </c>
+      <c r="O11" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="12" s="32" spans="1:15">
+      <c r="A12" s="40" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="43" t="s">
+        <v>72</v>
+      </c>
+      <c r="E12" s="62" t="n">
+        <v>2</v>
+      </c>
+      <c r="F12" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="H12" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="I12" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="J12" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="K12" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="L12" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="M12" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="N12" s="45" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="O12" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="13" s="32" spans="1:15">
+      <c r="A13" s="40" t="s"/>
+      <c r="B13" s="41" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="J8" s="64" t="s">
-        <v>46</v>
-      </c>
-      <c r="K8" s="64" t="s">
-        <v>49</v>
-      </c>
-      <c r="L8" s="67" t="s">
-        <v>39</v>
-      </c>
-      <c r="M8" s="67" t="s">
-        <v>50</v>
-      </c>
-      <c r="N8" s="68" t="n">
-        <v>2.16</v>
-      </c>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="9" s="32" spans="1:14">
-      <c r="A9" s="62" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" s="63" t="s"/>
-      <c r="C9" s="64" t="s">
-        <v>52</v>
-      </c>
-      <c r="D9" s="65" t="s">
+      <c r="D13" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="E13" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="G13" s="40" t="s">
+        <v>80</v>
+      </c>
+      <c r="H13" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="I13" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="J13" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="E9" s="66" t="n">
-        <v>1</v>
-      </c>
-      <c r="F9" s="62" t="s">
-        <v>46</v>
-      </c>
-      <c r="G9" s="62" t="s">
-        <v>54</v>
-      </c>
-      <c r="H9" s="62" t="s">
-        <v>39</v>
-      </c>
-      <c r="I9" s="62" t="s">
-        <v>55</v>
-      </c>
-      <c r="J9" s="62" t="s">
-        <v>46</v>
-      </c>
-      <c r="K9" s="62" t="s">
-        <v>56</v>
-      </c>
-      <c r="L9" s="67" t="s">
-        <v>39</v>
-      </c>
-      <c r="M9" s="67" t="s">
-        <v>57</v>
-      </c>
-      <c r="N9" s="68" t="n">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="10" s="32" spans="1:14">
-      <c r="A10" s="62" t="s">
-        <v>58</v>
-      </c>
-      <c r="B10" s="63" t="s">
-        <v>59</v>
-      </c>
-      <c r="C10" s="64" t="s">
-        <v>60</v>
-      </c>
-      <c r="D10" s="65" t="s">
-        <v>61</v>
-      </c>
-      <c r="E10" s="66" t="n">
-        <v>2</v>
-      </c>
-      <c r="F10" s="64" t="s">
-        <v>46</v>
-      </c>
-      <c r="G10" s="64" t="s">
-        <v>62</v>
-      </c>
-      <c r="H10" s="64" t="s">
-        <v>39</v>
-      </c>
-      <c r="I10" s="64" t="s">
-        <v>63</v>
-      </c>
-      <c r="J10" s="64" t="s">
-        <v>46</v>
-      </c>
-      <c r="K10" s="64" t="s">
-        <v>64</v>
-      </c>
-      <c r="L10" s="67" t="s">
-        <v>39</v>
-      </c>
-      <c r="M10" s="67" t="s">
-        <v>65</v>
-      </c>
-      <c r="N10" s="68" t="n">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="11" s="32" spans="1:14">
-      <c r="A11" s="62" t="s"/>
-      <c r="B11" s="63" t="s">
-        <v>66</v>
-      </c>
-      <c r="C11" s="64" t="s">
-        <v>67</v>
-      </c>
-      <c r="D11" s="65" t="s">
-        <v>68</v>
-      </c>
-      <c r="E11" s="66" t="n">
+      <c r="K13" s="40" t="s">
+        <v>82</v>
+      </c>
+      <c r="L13" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="M13" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="N13" s="45" t="n">
         <v>0</v>
       </c>
-      <c r="F11" s="62" t="s">
-        <v>69</v>
-      </c>
-      <c r="G11" s="62" t="s">
-        <v>70</v>
-      </c>
-      <c r="H11" s="62" t="s">
-        <v>39</v>
-      </c>
-      <c r="I11" s="62" t="s">
-        <v>71</v>
-      </c>
-      <c r="J11" s="62" t="s">
-        <v>72</v>
-      </c>
-      <c r="K11" s="62" t="s">
-        <v>73</v>
-      </c>
-      <c r="L11" s="67" t="s">
-        <v>39</v>
-      </c>
-      <c r="M11" s="67" t="s">
-        <v>74</v>
-      </c>
-      <c r="N11" s="68" t="n">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="12" s="32" spans="1:14">
-      <c r="A12" s="62" t="s"/>
-      <c r="B12" s="63" t="s">
-        <v>75</v>
-      </c>
-      <c r="C12" s="64" t="s">
-        <v>67</v>
-      </c>
-      <c r="D12" s="65" t="s">
-        <v>76</v>
-      </c>
-      <c r="E12" s="66" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" s="64" t="s">
-        <v>72</v>
-      </c>
-      <c r="G12" s="64" t="s">
-        <v>77</v>
-      </c>
-      <c r="H12" s="64" t="s">
-        <v>39</v>
-      </c>
-      <c r="I12" s="64" t="s">
-        <v>78</v>
-      </c>
-      <c r="J12" s="64" t="s">
-        <v>79</v>
-      </c>
-      <c r="K12" s="64" t="s">
-        <v>80</v>
-      </c>
-      <c r="L12" s="67" t="s">
-        <v>39</v>
-      </c>
-      <c r="M12" s="67" t="s">
-        <v>81</v>
-      </c>
-      <c r="N12" s="68" t="n">
-        <v>1.55</v>
-      </c>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="13" s="32" spans="1:14">
-      <c r="A13" s="62" t="s">
-        <v>82</v>
-      </c>
-      <c r="B13" s="63" t="s"/>
-      <c r="C13" s="64" t="s">
-        <v>83</v>
-      </c>
-      <c r="D13" s="65" t="s">
-        <v>84</v>
-      </c>
-      <c r="E13" s="66" t="n">
-        <v>5</v>
-      </c>
-      <c r="F13" s="62" t="s">
-        <v>37</v>
-      </c>
-      <c r="G13" s="62" t="s">
-        <v>85</v>
-      </c>
-      <c r="H13" s="62" t="s">
-        <v>39</v>
-      </c>
-      <c r="I13" s="62" t="s">
-        <v>86</v>
-      </c>
-      <c r="J13" s="62" t="s">
-        <v>37</v>
-      </c>
-      <c r="K13" s="62" t="s">
-        <v>87</v>
-      </c>
-      <c r="L13" s="67" t="s">
-        <v>39</v>
-      </c>
-      <c r="M13" s="67" t="s">
-        <v>88</v>
-      </c>
-      <c r="N13" s="68" t="n">
-        <v>2.2</v>
-      </c>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="14" s="32" spans="1:14">
+      <c r="O13" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="14" s="32" spans="1:15">
       <c r="A14" s="40" t="s"/>
       <c r="B14" s="41" t="s"/>
       <c r="C14" s="42" t="s"/>
       <c r="D14" s="43" t="s"/>
-      <c r="E14" s="69" t="s"/>
+      <c r="E14" s="62" t="s"/>
       <c r="F14" s="42" t="s"/>
       <c r="G14" s="42" t="s"/>
       <c r="H14" s="42" t="s"/>
@@ -2799,13 +2765,14 @@
       <c r="L14" s="44" t="s"/>
       <c r="M14" s="44" t="s"/>
       <c r="N14" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="15" s="32" spans="1:14">
+      <c r="O14" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="15" s="32" spans="1:15">
       <c r="A15" s="40" t="s"/>
       <c r="B15" s="41" t="s"/>
       <c r="C15" s="42" t="s"/>
       <c r="D15" s="43" t="s"/>
-      <c r="E15" s="69" t="s"/>
+      <c r="E15" s="62" t="s"/>
       <c r="F15" s="40" t="s"/>
       <c r="G15" s="40" t="s"/>
       <c r="H15" s="40" t="s"/>
@@ -2815,13 +2782,14 @@
       <c r="L15" s="44" t="s"/>
       <c r="M15" s="44" t="s"/>
       <c r="N15" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="16" s="32" spans="1:14">
+      <c r="O15" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="16" s="32" spans="1:15">
       <c r="A16" s="40" t="s"/>
       <c r="B16" s="41" t="s"/>
       <c r="C16" s="42" t="s"/>
       <c r="D16" s="43" t="s"/>
-      <c r="E16" s="69" t="s"/>
+      <c r="E16" s="62" t="s"/>
       <c r="F16" s="42" t="s"/>
       <c r="G16" s="42" t="s"/>
       <c r="H16" s="42" t="s"/>
@@ -2831,13 +2799,14 @@
       <c r="L16" s="44" t="s"/>
       <c r="M16" s="44" t="s"/>
       <c r="N16" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="17" s="32" spans="1:14">
+      <c r="O16" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="17" s="32" spans="1:15">
       <c r="A17" s="40" t="s"/>
       <c r="B17" s="41" t="s"/>
       <c r="C17" s="42" t="s"/>
       <c r="D17" s="43" t="s"/>
-      <c r="E17" s="69" t="s"/>
+      <c r="E17" s="62" t="s"/>
       <c r="F17" s="40" t="s"/>
       <c r="G17" s="40" t="s"/>
       <c r="H17" s="40" t="s"/>
@@ -2847,13 +2816,14 @@
       <c r="L17" s="44" t="s"/>
       <c r="M17" s="44" t="s"/>
       <c r="N17" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="18" s="32" spans="1:14">
+      <c r="O17" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="18" s="32" spans="1:15">
       <c r="A18" s="40" t="s"/>
       <c r="B18" s="41" t="s"/>
       <c r="C18" s="42" t="s"/>
       <c r="D18" s="43" t="s"/>
-      <c r="E18" s="69" t="s"/>
+      <c r="E18" s="62" t="s"/>
       <c r="F18" s="42" t="s"/>
       <c r="G18" s="42" t="s"/>
       <c r="H18" s="42" t="s"/>
@@ -2863,13 +2833,14 @@
       <c r="L18" s="44" t="s"/>
       <c r="M18" s="44" t="s"/>
       <c r="N18" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="19" s="32" spans="1:14">
+      <c r="O18" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="19" s="32" spans="1:15">
       <c r="A19" s="40" t="s"/>
       <c r="B19" s="41" t="s"/>
       <c r="C19" s="42" t="s"/>
       <c r="D19" s="43" t="s"/>
-      <c r="E19" s="69" t="s"/>
+      <c r="E19" s="62" t="s"/>
       <c r="F19" s="40" t="s"/>
       <c r="G19" s="40" t="s"/>
       <c r="H19" s="40" t="s"/>
@@ -2879,13 +2850,14 @@
       <c r="L19" s="44" t="s"/>
       <c r="M19" s="44" t="s"/>
       <c r="N19" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="20" s="32" spans="1:14">
+      <c r="O19" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="20" s="32" spans="1:15">
       <c r="A20" s="40" t="s"/>
       <c r="B20" s="41" t="s"/>
       <c r="C20" s="42" t="s"/>
       <c r="D20" s="43" t="s"/>
-      <c r="E20" s="69" t="s"/>
+      <c r="E20" s="62" t="s"/>
       <c r="F20" s="42" t="s"/>
       <c r="G20" s="42" t="s"/>
       <c r="H20" s="42" t="s"/>
@@ -2895,13 +2867,14 @@
       <c r="L20" s="44" t="s"/>
       <c r="M20" s="44" t="s"/>
       <c r="N20" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="21" s="32" spans="1:14">
+      <c r="O20" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="21" s="32" spans="1:15">
       <c r="A21" s="40" t="s"/>
       <c r="B21" s="41" t="s"/>
       <c r="C21" s="42" t="s"/>
       <c r="D21" s="43" t="s"/>
-      <c r="E21" s="69" t="s"/>
+      <c r="E21" s="62" t="s"/>
       <c r="F21" s="40" t="s"/>
       <c r="G21" s="40" t="s"/>
       <c r="H21" s="40" t="s"/>
@@ -2911,13 +2884,14 @@
       <c r="L21" s="44" t="s"/>
       <c r="M21" s="44" t="s"/>
       <c r="N21" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="22" s="32" spans="1:14">
+      <c r="O21" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="22" s="32" spans="1:15">
       <c r="A22" s="40" t="s"/>
       <c r="B22" s="41" t="s"/>
       <c r="C22" s="42" t="s"/>
       <c r="D22" s="43" t="s"/>
-      <c r="E22" s="69" t="s"/>
+      <c r="E22" s="62" t="s"/>
       <c r="F22" s="42" t="s"/>
       <c r="G22" s="42" t="s"/>
       <c r="H22" s="42" t="s"/>
@@ -2927,13 +2901,14 @@
       <c r="L22" s="44" t="s"/>
       <c r="M22" s="44" t="s"/>
       <c r="N22" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="23" s="32" spans="1:14">
+      <c r="O22" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="23" s="32" spans="1:15">
       <c r="A23" s="40" t="s"/>
       <c r="B23" s="41" t="s"/>
       <c r="C23" s="42" t="s"/>
       <c r="D23" s="43" t="s"/>
-      <c r="E23" s="69" t="s"/>
+      <c r="E23" s="62" t="s"/>
       <c r="F23" s="40" t="s"/>
       <c r="G23" s="40" t="s"/>
       <c r="H23" s="40" t="s"/>
@@ -2943,13 +2918,14 @@
       <c r="L23" s="44" t="s"/>
       <c r="M23" s="44" t="s"/>
       <c r="N23" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="24" s="32" spans="1:14">
+      <c r="O23" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="24" s="32" spans="1:15">
       <c r="A24" s="40" t="s"/>
       <c r="B24" s="41" t="s"/>
       <c r="C24" s="42" t="s"/>
       <c r="D24" s="43" t="s"/>
-      <c r="E24" s="69" t="s"/>
+      <c r="E24" s="62" t="s"/>
       <c r="F24" s="42" t="s"/>
       <c r="G24" s="42" t="s"/>
       <c r="H24" s="42" t="s"/>
@@ -2959,13 +2935,14 @@
       <c r="L24" s="44" t="s"/>
       <c r="M24" s="44" t="s"/>
       <c r="N24" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="25" s="32" spans="1:14">
+      <c r="O24" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="25" s="32" spans="1:15">
       <c r="A25" s="40" t="s"/>
       <c r="B25" s="41" t="s"/>
       <c r="C25" s="42" t="s"/>
       <c r="D25" s="43" t="s"/>
-      <c r="E25" s="69" t="s"/>
+      <c r="E25" s="62" t="s"/>
       <c r="F25" s="40" t="s"/>
       <c r="G25" s="40" t="s"/>
       <c r="H25" s="40" t="s"/>
@@ -2975,13 +2952,14 @@
       <c r="L25" s="44" t="s"/>
       <c r="M25" s="44" t="s"/>
       <c r="N25" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="26" s="32" spans="1:14">
+      <c r="O25" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="26" s="32" spans="1:15">
       <c r="A26" s="40" t="s"/>
       <c r="B26" s="41" t="s"/>
       <c r="C26" s="42" t="s"/>
       <c r="D26" s="43" t="s"/>
-      <c r="E26" s="69" t="s"/>
+      <c r="E26" s="62" t="s"/>
       <c r="F26" s="42" t="s"/>
       <c r="G26" s="42" t="s"/>
       <c r="H26" s="42" t="s"/>
@@ -2991,13 +2969,14 @@
       <c r="L26" s="44" t="s"/>
       <c r="M26" s="44" t="s"/>
       <c r="N26" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="27" s="32" spans="1:14">
+      <c r="O26" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="27" s="32" spans="1:15">
       <c r="A27" s="40" t="s"/>
       <c r="B27" s="41" t="s"/>
       <c r="C27" s="42" t="s"/>
       <c r="D27" s="43" t="s"/>
-      <c r="E27" s="69" t="s"/>
+      <c r="E27" s="62" t="s"/>
       <c r="F27" s="40" t="s"/>
       <c r="G27" s="40" t="s"/>
       <c r="H27" s="40" t="s"/>
@@ -3007,13 +2986,14 @@
       <c r="L27" s="44" t="s"/>
       <c r="M27" s="44" t="s"/>
       <c r="N27" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="28" s="32" spans="1:14">
+      <c r="O27" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="28" s="32" spans="1:15">
       <c r="A28" s="40" t="s"/>
       <c r="B28" s="41" t="s"/>
       <c r="C28" s="42" t="s"/>
       <c r="D28" s="43" t="s"/>
-      <c r="E28" s="69" t="s"/>
+      <c r="E28" s="62" t="s"/>
       <c r="F28" s="42" t="s"/>
       <c r="G28" s="42" t="s"/>
       <c r="H28" s="42" t="s"/>
@@ -3023,13 +3003,14 @@
       <c r="L28" s="44" t="s"/>
       <c r="M28" s="44" t="s"/>
       <c r="N28" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="29" s="32" spans="1:14">
+      <c r="O28" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="29" s="32" spans="1:15">
       <c r="A29" s="40" t="s"/>
       <c r="B29" s="41" t="s"/>
       <c r="C29" s="42" t="s"/>
       <c r="D29" s="43" t="s"/>
-      <c r="E29" s="69" t="s"/>
+      <c r="E29" s="62" t="s"/>
       <c r="F29" s="40" t="s"/>
       <c r="G29" s="40" t="s"/>
       <c r="H29" s="40" t="s"/>
@@ -3039,13 +3020,14 @@
       <c r="L29" s="44" t="s"/>
       <c r="M29" s="44" t="s"/>
       <c r="N29" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="30" s="32" spans="1:14">
+      <c r="O29" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="30" s="32" spans="1:15">
       <c r="A30" s="40" t="s"/>
       <c r="B30" s="41" t="s"/>
       <c r="C30" s="42" t="s"/>
       <c r="D30" s="43" t="s"/>
-      <c r="E30" s="69" t="s"/>
+      <c r="E30" s="62" t="s"/>
       <c r="F30" s="42" t="s"/>
       <c r="G30" s="42" t="s"/>
       <c r="H30" s="42" t="s"/>
@@ -3055,13 +3037,14 @@
       <c r="L30" s="44" t="s"/>
       <c r="M30" s="44" t="s"/>
       <c r="N30" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="31" s="32" spans="1:14">
+      <c r="O30" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="31" s="32" spans="1:15">
       <c r="A31" s="40" t="s"/>
       <c r="B31" s="41" t="s"/>
       <c r="C31" s="42" t="s"/>
       <c r="D31" s="43" t="s"/>
-      <c r="E31" s="69" t="s"/>
+      <c r="E31" s="62" t="s"/>
       <c r="F31" s="40" t="s"/>
       <c r="G31" s="40" t="s"/>
       <c r="H31" s="40" t="s"/>
@@ -3071,13 +3054,14 @@
       <c r="L31" s="44" t="s"/>
       <c r="M31" s="44" t="s"/>
       <c r="N31" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="32" s="32" spans="1:14">
+      <c r="O31" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="32" s="32" spans="1:15">
       <c r="A32" s="40" t="s"/>
       <c r="B32" s="41" t="s"/>
       <c r="C32" s="42" t="s"/>
       <c r="D32" s="43" t="s"/>
-      <c r="E32" s="69" t="s"/>
+      <c r="E32" s="62" t="s"/>
       <c r="F32" s="42" t="s"/>
       <c r="G32" s="42" t="s"/>
       <c r="H32" s="42" t="s"/>
@@ -3087,13 +3071,14 @@
       <c r="L32" s="44" t="s"/>
       <c r="M32" s="44" t="s"/>
       <c r="N32" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="33" s="32" spans="1:14">
+      <c r="O32" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="33" s="32" spans="1:15">
       <c r="A33" s="40" t="s"/>
       <c r="B33" s="41" t="s"/>
       <c r="C33" s="42" t="s"/>
       <c r="D33" s="43" t="s"/>
-      <c r="E33" s="69" t="s"/>
+      <c r="E33" s="62" t="s"/>
       <c r="F33" s="40" t="s"/>
       <c r="G33" s="40" t="s"/>
       <c r="H33" s="40" t="s"/>
@@ -3103,13 +3088,14 @@
       <c r="L33" s="44" t="s"/>
       <c r="M33" s="44" t="s"/>
       <c r="N33" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="34" s="32" spans="1:14">
+      <c r="O33" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="34" s="32" spans="1:15">
       <c r="A34" s="40" t="s"/>
       <c r="B34" s="41" t="s"/>
       <c r="C34" s="42" t="s"/>
       <c r="D34" s="43" t="s"/>
-      <c r="E34" s="69" t="s"/>
+      <c r="E34" s="62" t="s"/>
       <c r="F34" s="42" t="s"/>
       <c r="G34" s="42" t="s"/>
       <c r="H34" s="42" t="s"/>
@@ -3119,13 +3105,14 @@
       <c r="L34" s="44" t="s"/>
       <c r="M34" s="44" t="s"/>
       <c r="N34" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="35" s="32" spans="1:14">
+      <c r="O34" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="35" s="32" spans="1:15">
       <c r="A35" s="40" t="s"/>
       <c r="B35" s="41" t="s"/>
       <c r="C35" s="42" t="s"/>
       <c r="D35" s="43" t="s"/>
-      <c r="E35" s="69" t="s"/>
+      <c r="E35" s="62" t="s"/>
       <c r="F35" s="40" t="s"/>
       <c r="G35" s="40" t="s"/>
       <c r="H35" s="40" t="s"/>
@@ -3135,13 +3122,14 @@
       <c r="L35" s="44" t="s"/>
       <c r="M35" s="44" t="s"/>
       <c r="N35" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="36" s="32" spans="1:14">
+      <c r="O35" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="36" s="32" spans="1:15">
       <c r="A36" s="40" t="s"/>
       <c r="B36" s="41" t="s"/>
       <c r="C36" s="42" t="s"/>
       <c r="D36" s="43" t="s"/>
-      <c r="E36" s="69" t="s"/>
+      <c r="E36" s="62" t="s"/>
       <c r="F36" s="42" t="s"/>
       <c r="G36" s="42" t="s"/>
       <c r="H36" s="42" t="s"/>
@@ -3151,13 +3139,14 @@
       <c r="L36" s="44" t="s"/>
       <c r="M36" s="44" t="s"/>
       <c r="N36" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="37" s="32" spans="1:14">
+      <c r="O36" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="37" s="32" spans="1:15">
       <c r="A37" s="40" t="s"/>
       <c r="B37" s="41" t="s"/>
       <c r="C37" s="42" t="s"/>
       <c r="D37" s="43" t="s"/>
-      <c r="E37" s="69" t="s"/>
+      <c r="E37" s="62" t="s"/>
       <c r="F37" s="40" t="s"/>
       <c r="G37" s="40" t="s"/>
       <c r="H37" s="40" t="s"/>
@@ -3167,13 +3156,14 @@
       <c r="L37" s="44" t="s"/>
       <c r="M37" s="44" t="s"/>
       <c r="N37" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="38" s="32" spans="1:14">
+      <c r="O37" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="38" s="32" spans="1:15">
       <c r="A38" s="40" t="s"/>
       <c r="B38" s="41" t="s"/>
       <c r="C38" s="42" t="s"/>
       <c r="D38" s="43" t="s"/>
-      <c r="E38" s="69" t="s"/>
+      <c r="E38" s="62" t="s"/>
       <c r="F38" s="42" t="s"/>
       <c r="G38" s="42" t="s"/>
       <c r="H38" s="42" t="s"/>
@@ -3183,13 +3173,14 @@
       <c r="L38" s="44" t="s"/>
       <c r="M38" s="44" t="s"/>
       <c r="N38" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="39" s="32" spans="1:14">
+      <c r="O38" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="39" s="32" spans="1:15">
       <c r="A39" s="40" t="s"/>
       <c r="B39" s="41" t="s"/>
       <c r="C39" s="42" t="s"/>
       <c r="D39" s="43" t="s"/>
-      <c r="E39" s="69" t="s"/>
+      <c r="E39" s="62" t="s"/>
       <c r="F39" s="40" t="s"/>
       <c r="G39" s="40" t="s"/>
       <c r="H39" s="40" t="s"/>
@@ -3199,13 +3190,14 @@
       <c r="L39" s="44" t="s"/>
       <c r="M39" s="44" t="s"/>
       <c r="N39" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="40" s="32" spans="1:14">
+      <c r="O39" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="40" s="32" spans="1:15">
       <c r="A40" s="40" t="s"/>
       <c r="B40" s="41" t="s"/>
       <c r="C40" s="42" t="s"/>
       <c r="D40" s="43" t="s"/>
-      <c r="E40" s="69" t="s"/>
+      <c r="E40" s="62" t="s"/>
       <c r="F40" s="42" t="s"/>
       <c r="G40" s="42" t="s"/>
       <c r="H40" s="42" t="s"/>
@@ -3215,13 +3207,14 @@
       <c r="L40" s="44" t="s"/>
       <c r="M40" s="44" t="s"/>
       <c r="N40" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="41" s="32" spans="1:14">
+      <c r="O40" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="41" s="32" spans="1:15">
       <c r="A41" s="40" t="s"/>
       <c r="B41" s="41" t="s"/>
       <c r="C41" s="42" t="s"/>
       <c r="D41" s="43" t="s"/>
-      <c r="E41" s="69" t="s"/>
+      <c r="E41" s="62" t="s"/>
       <c r="F41" s="40" t="s"/>
       <c r="G41" s="40" t="s"/>
       <c r="H41" s="40" t="s"/>
@@ -3231,13 +3224,14 @@
       <c r="L41" s="44" t="s"/>
       <c r="M41" s="44" t="s"/>
       <c r="N41" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="42" s="32" spans="1:14">
+      <c r="O41" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="42" s="32" spans="1:15">
       <c r="A42" s="40" t="s"/>
       <c r="B42" s="41" t="s"/>
       <c r="C42" s="42" t="s"/>
       <c r="D42" s="43" t="s"/>
-      <c r="E42" s="69" t="s"/>
+      <c r="E42" s="62" t="s"/>
       <c r="F42" s="42" t="s"/>
       <c r="G42" s="42" t="s"/>
       <c r="H42" s="42" t="s"/>
@@ -3247,13 +3241,14 @@
       <c r="L42" s="44" t="s"/>
       <c r="M42" s="44" t="s"/>
       <c r="N42" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="43" s="32" spans="1:14">
+      <c r="O42" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="43" s="32" spans="1:15">
       <c r="A43" s="40" t="s"/>
       <c r="B43" s="41" t="s"/>
       <c r="C43" s="42" t="s"/>
       <c r="D43" s="43" t="s"/>
-      <c r="E43" s="69" t="s"/>
+      <c r="E43" s="62" t="s"/>
       <c r="F43" s="40" t="s"/>
       <c r="G43" s="40" t="s"/>
       <c r="H43" s="40" t="s"/>
@@ -3263,13 +3258,14 @@
       <c r="L43" s="44" t="s"/>
       <c r="M43" s="44" t="s"/>
       <c r="N43" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="44" s="32" spans="1:14">
+      <c r="O43" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="44" s="32" spans="1:15">
       <c r="A44" s="40" t="s"/>
       <c r="B44" s="41" t="s"/>
       <c r="C44" s="42" t="s"/>
       <c r="D44" s="43" t="s"/>
-      <c r="E44" s="69" t="s"/>
+      <c r="E44" s="62" t="s"/>
       <c r="F44" s="42" t="s"/>
       <c r="G44" s="42" t="s"/>
       <c r="H44" s="42" t="s"/>
@@ -3279,13 +3275,14 @@
       <c r="L44" s="44" t="s"/>
       <c r="M44" s="44" t="s"/>
       <c r="N44" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="45" s="32" spans="1:14">
+      <c r="O44" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="45" s="32" spans="1:15">
       <c r="A45" s="40" t="s"/>
       <c r="B45" s="41" t="s"/>
       <c r="C45" s="42" t="s"/>
       <c r="D45" s="43" t="s"/>
-      <c r="E45" s="69" t="s"/>
+      <c r="E45" s="62" t="s"/>
       <c r="F45" s="40" t="s"/>
       <c r="G45" s="40" t="s"/>
       <c r="H45" s="40" t="s"/>
@@ -3295,13 +3292,14 @@
       <c r="L45" s="44" t="s"/>
       <c r="M45" s="44" t="s"/>
       <c r="N45" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="46" s="32" spans="1:14">
+      <c r="O45" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="46" s="32" spans="1:15">
       <c r="A46" s="40" t="s"/>
       <c r="B46" s="41" t="s"/>
       <c r="C46" s="42" t="s"/>
       <c r="D46" s="43" t="s"/>
-      <c r="E46" s="69" t="s"/>
+      <c r="E46" s="62" t="s"/>
       <c r="F46" s="42" t="s"/>
       <c r="G46" s="42" t="s"/>
       <c r="H46" s="42" t="s"/>
@@ -3311,13 +3309,14 @@
       <c r="L46" s="44" t="s"/>
       <c r="M46" s="44" t="s"/>
       <c r="N46" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="47" s="32" spans="1:14">
+      <c r="O46" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="47" s="32" spans="1:15">
       <c r="A47" s="40" t="s"/>
       <c r="B47" s="41" t="s"/>
       <c r="C47" s="42" t="s"/>
       <c r="D47" s="43" t="s"/>
-      <c r="E47" s="69" t="s"/>
+      <c r="E47" s="62" t="s"/>
       <c r="F47" s="40" t="s"/>
       <c r="G47" s="40" t="s"/>
       <c r="H47" s="40" t="s"/>
@@ -3327,13 +3326,14 @@
       <c r="L47" s="44" t="s"/>
       <c r="M47" s="44" t="s"/>
       <c r="N47" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="48" s="32" spans="1:14">
+      <c r="O47" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="48" s="32" spans="1:15">
       <c r="A48" s="40" t="s"/>
       <c r="B48" s="41" t="s"/>
       <c r="C48" s="42" t="s"/>
       <c r="D48" s="43" t="s"/>
-      <c r="E48" s="69" t="s"/>
+      <c r="E48" s="62" t="s"/>
       <c r="F48" s="42" t="s"/>
       <c r="G48" s="42" t="s"/>
       <c r="H48" s="42" t="s"/>
@@ -3343,13 +3343,14 @@
       <c r="L48" s="44" t="s"/>
       <c r="M48" s="44" t="s"/>
       <c r="N48" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="49" s="32" spans="1:14">
+      <c r="O48" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="49" s="32" spans="1:15">
       <c r="A49" s="40" t="s"/>
       <c r="B49" s="41" t="s"/>
       <c r="C49" s="42" t="s"/>
       <c r="D49" s="43" t="s"/>
-      <c r="E49" s="69" t="s"/>
+      <c r="E49" s="62" t="s"/>
       <c r="F49" s="40" t="s"/>
       <c r="G49" s="40" t="s"/>
       <c r="H49" s="40" t="s"/>
@@ -3359,13 +3360,14 @@
       <c r="L49" s="44" t="s"/>
       <c r="M49" s="44" t="s"/>
       <c r="N49" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="50" s="32" spans="1:14">
+      <c r="O49" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="50" s="32" spans="1:15">
       <c r="A50" s="40" t="s"/>
       <c r="B50" s="41" t="s"/>
       <c r="C50" s="42" t="s"/>
       <c r="D50" s="43" t="s"/>
-      <c r="E50" s="69" t="s"/>
+      <c r="E50" s="62" t="s"/>
       <c r="F50" s="42" t="s"/>
       <c r="G50" s="42" t="s"/>
       <c r="H50" s="42" t="s"/>
@@ -3375,13 +3377,14 @@
       <c r="L50" s="44" t="s"/>
       <c r="M50" s="44" t="s"/>
       <c r="N50" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="51" s="32" spans="1:14">
+      <c r="O50" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="51" s="32" spans="1:15">
       <c r="A51" s="40" t="s"/>
       <c r="B51" s="41" t="s"/>
       <c r="C51" s="42" t="s"/>
       <c r="D51" s="43" t="s"/>
-      <c r="E51" s="69" t="s"/>
+      <c r="E51" s="62" t="s"/>
       <c r="F51" s="40" t="s"/>
       <c r="G51" s="40" t="s"/>
       <c r="H51" s="40" t="s"/>
@@ -3391,13 +3394,14 @@
       <c r="L51" s="44" t="s"/>
       <c r="M51" s="44" t="s"/>
       <c r="N51" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="52" s="32" spans="1:14">
+      <c r="O51" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="52" s="32" spans="1:15">
       <c r="A52" s="40" t="s"/>
       <c r="B52" s="41" t="s"/>
       <c r="C52" s="42" t="s"/>
       <c r="D52" s="43" t="s"/>
-      <c r="E52" s="69" t="s"/>
+      <c r="E52" s="62" t="s"/>
       <c r="F52" s="42" t="s"/>
       <c r="G52" s="42" t="s"/>
       <c r="H52" s="42" t="s"/>
@@ -3407,13 +3411,14 @@
       <c r="L52" s="44" t="s"/>
       <c r="M52" s="44" t="s"/>
       <c r="N52" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="53" s="32" spans="1:14">
+      <c r="O52" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="53" s="32" spans="1:15">
       <c r="A53" s="40" t="s"/>
       <c r="B53" s="41" t="s"/>
       <c r="C53" s="42" t="s"/>
       <c r="D53" s="43" t="s"/>
-      <c r="E53" s="69" t="s"/>
+      <c r="E53" s="62" t="s"/>
       <c r="F53" s="40" t="s"/>
       <c r="G53" s="40" t="s"/>
       <c r="H53" s="40" t="s"/>
@@ -3423,13 +3428,14 @@
       <c r="L53" s="44" t="s"/>
       <c r="M53" s="44" t="s"/>
       <c r="N53" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="54" s="32" spans="1:14">
+      <c r="O53" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="54" s="32" spans="1:15">
       <c r="A54" s="40" t="s"/>
       <c r="B54" s="41" t="s"/>
       <c r="C54" s="42" t="s"/>
       <c r="D54" s="43" t="s"/>
-      <c r="E54" s="69" t="s"/>
+      <c r="E54" s="62" t="s"/>
       <c r="F54" s="42" t="s"/>
       <c r="G54" s="42" t="s"/>
       <c r="H54" s="42" t="s"/>
@@ -3439,13 +3445,14 @@
       <c r="L54" s="44" t="s"/>
       <c r="M54" s="44" t="s"/>
       <c r="N54" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="55" s="32" spans="1:14">
+      <c r="O54" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="55" s="32" spans="1:15">
       <c r="A55" s="40" t="s"/>
       <c r="B55" s="41" t="s"/>
       <c r="C55" s="42" t="s"/>
       <c r="D55" s="43" t="s"/>
-      <c r="E55" s="69" t="s"/>
+      <c r="E55" s="62" t="s"/>
       <c r="F55" s="40" t="s"/>
       <c r="G55" s="40" t="s"/>
       <c r="H55" s="40" t="s"/>
@@ -3455,13 +3462,14 @@
       <c r="L55" s="44" t="s"/>
       <c r="M55" s="44" t="s"/>
       <c r="N55" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="56" s="32" spans="1:14">
+      <c r="O55" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="56" s="32" spans="1:15">
       <c r="A56" s="40" t="s"/>
       <c r="B56" s="41" t="s"/>
       <c r="C56" s="42" t="s"/>
       <c r="D56" s="43" t="s"/>
-      <c r="E56" s="69" t="s"/>
+      <c r="E56" s="62" t="s"/>
       <c r="F56" s="42" t="s"/>
       <c r="G56" s="42" t="s"/>
       <c r="H56" s="42" t="s"/>
@@ -3471,13 +3479,14 @@
       <c r="L56" s="44" t="s"/>
       <c r="M56" s="44" t="s"/>
       <c r="N56" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="57" s="32" spans="1:14">
+      <c r="O56" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="57" s="32" spans="1:15">
       <c r="A57" s="40" t="s"/>
       <c r="B57" s="41" t="s"/>
       <c r="C57" s="42" t="s"/>
       <c r="D57" s="43" t="s"/>
-      <c r="E57" s="69" t="s"/>
+      <c r="E57" s="62" t="s"/>
       <c r="F57" s="40" t="s"/>
       <c r="G57" s="40" t="s"/>
       <c r="H57" s="40" t="s"/>
@@ -3487,13 +3496,14 @@
       <c r="L57" s="44" t="s"/>
       <c r="M57" s="44" t="s"/>
       <c r="N57" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="58" s="32" spans="1:14">
+      <c r="O57" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="58" s="32" spans="1:15">
       <c r="A58" s="40" t="s"/>
       <c r="B58" s="41" t="s"/>
       <c r="C58" s="42" t="s"/>
       <c r="D58" s="43" t="s"/>
-      <c r="E58" s="69" t="s"/>
+      <c r="E58" s="62" t="s"/>
       <c r="F58" s="42" t="s"/>
       <c r="G58" s="42" t="s"/>
       <c r="H58" s="42" t="s"/>
@@ -3503,13 +3513,14 @@
       <c r="L58" s="44" t="s"/>
       <c r="M58" s="44" t="s"/>
       <c r="N58" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="59" s="32" spans="1:14">
+      <c r="O58" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="59" s="32" spans="1:15">
       <c r="A59" s="40" t="s"/>
       <c r="B59" s="41" t="s"/>
       <c r="C59" s="42" t="s"/>
       <c r="D59" s="43" t="s"/>
-      <c r="E59" s="69" t="s"/>
+      <c r="E59" s="62" t="s"/>
       <c r="F59" s="40" t="s"/>
       <c r="G59" s="40" t="s"/>
       <c r="H59" s="40" t="s"/>
@@ -3519,13 +3530,14 @@
       <c r="L59" s="44" t="s"/>
       <c r="M59" s="44" t="s"/>
       <c r="N59" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="60" s="32" spans="1:14">
+      <c r="O59" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="60" s="32" spans="1:15">
       <c r="A60" s="40" t="s"/>
       <c r="B60" s="41" t="s"/>
       <c r="C60" s="42" t="s"/>
       <c r="D60" s="43" t="s"/>
-      <c r="E60" s="69" t="s"/>
+      <c r="E60" s="62" t="s"/>
       <c r="F60" s="42" t="s"/>
       <c r="G60" s="42" t="s"/>
       <c r="H60" s="42" t="s"/>
@@ -3535,13 +3547,14 @@
       <c r="L60" s="44" t="s"/>
       <c r="M60" s="44" t="s"/>
       <c r="N60" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="61" s="32" spans="1:14">
+      <c r="O60" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="61" s="32" spans="1:15">
       <c r="A61" s="40" t="s"/>
       <c r="B61" s="41" t="s"/>
       <c r="C61" s="42" t="s"/>
       <c r="D61" s="43" t="s"/>
-      <c r="E61" s="69" t="s"/>
+      <c r="E61" s="62" t="s"/>
       <c r="F61" s="40" t="s"/>
       <c r="G61" s="40" t="s"/>
       <c r="H61" s="40" t="s"/>
@@ -3551,13 +3564,14 @@
       <c r="L61" s="44" t="s"/>
       <c r="M61" s="44" t="s"/>
       <c r="N61" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="62" s="32" spans="1:14">
+      <c r="O61" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="62" s="32" spans="1:15">
       <c r="A62" s="40" t="s"/>
       <c r="B62" s="41" t="s"/>
       <c r="C62" s="42" t="s"/>
       <c r="D62" s="43" t="s"/>
-      <c r="E62" s="69" t="s"/>
+      <c r="E62" s="62" t="s"/>
       <c r="F62" s="42" t="s"/>
       <c r="G62" s="42" t="s"/>
       <c r="H62" s="42" t="s"/>
@@ -3567,13 +3581,14 @@
       <c r="L62" s="44" t="s"/>
       <c r="M62" s="44" t="s"/>
       <c r="N62" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="63" s="32" spans="1:14">
+      <c r="O62" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="63" s="32" spans="1:15">
       <c r="A63" s="40" t="s"/>
       <c r="B63" s="41" t="s"/>
       <c r="C63" s="42" t="s"/>
       <c r="D63" s="43" t="s"/>
-      <c r="E63" s="69" t="s"/>
+      <c r="E63" s="62" t="s"/>
       <c r="F63" s="40" t="s"/>
       <c r="G63" s="40" t="s"/>
       <c r="H63" s="40" t="s"/>
@@ -3583,13 +3598,14 @@
       <c r="L63" s="44" t="s"/>
       <c r="M63" s="44" t="s"/>
       <c r="N63" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="64" s="32" spans="1:14">
+      <c r="O63" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="64" s="32" spans="1:15">
       <c r="A64" s="40" t="s"/>
       <c r="B64" s="41" t="s"/>
       <c r="C64" s="42" t="s"/>
       <c r="D64" s="43" t="s"/>
-      <c r="E64" s="69" t="s"/>
+      <c r="E64" s="62" t="s"/>
       <c r="F64" s="42" t="s"/>
       <c r="G64" s="42" t="s"/>
       <c r="H64" s="42" t="s"/>
@@ -3599,13 +3615,14 @@
       <c r="L64" s="44" t="s"/>
       <c r="M64" s="44" t="s"/>
       <c r="N64" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="65" s="32" spans="1:14">
+      <c r="O64" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="65" s="32" spans="1:15">
       <c r="A65" s="40" t="s"/>
       <c r="B65" s="41" t="s"/>
       <c r="C65" s="42" t="s"/>
       <c r="D65" s="43" t="s"/>
-      <c r="E65" s="69" t="s"/>
+      <c r="E65" s="62" t="s"/>
       <c r="F65" s="40" t="s"/>
       <c r="G65" s="40" t="s"/>
       <c r="H65" s="40" t="s"/>
@@ -3615,13 +3632,14 @@
       <c r="L65" s="44" t="s"/>
       <c r="M65" s="44" t="s"/>
       <c r="N65" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="66" s="32" spans="1:14">
+      <c r="O65" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="66" s="32" spans="1:15">
       <c r="A66" s="40" t="s"/>
       <c r="B66" s="41" t="s"/>
       <c r="C66" s="42" t="s"/>
       <c r="D66" s="43" t="s"/>
-      <c r="E66" s="69" t="s"/>
+      <c r="E66" s="62" t="s"/>
       <c r="F66" s="42" t="s"/>
       <c r="G66" s="42" t="s"/>
       <c r="H66" s="42" t="s"/>
@@ -3631,13 +3649,14 @@
       <c r="L66" s="44" t="s"/>
       <c r="M66" s="44" t="s"/>
       <c r="N66" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="67" s="32" spans="1:14">
+      <c r="O66" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="67" s="32" spans="1:15">
       <c r="A67" s="40" t="s"/>
       <c r="B67" s="41" t="s"/>
       <c r="C67" s="42" t="s"/>
       <c r="D67" s="43" t="s"/>
-      <c r="E67" s="69" t="s"/>
+      <c r="E67" s="62" t="s"/>
       <c r="F67" s="40" t="s"/>
       <c r="G67" s="40" t="s"/>
       <c r="H67" s="40" t="s"/>
@@ -3647,13 +3666,14 @@
       <c r="L67" s="44" t="s"/>
       <c r="M67" s="44" t="s"/>
       <c r="N67" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="68" s="32" spans="1:14">
+      <c r="O67" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="68" s="32" spans="1:15">
       <c r="A68" s="40" t="s"/>
       <c r="B68" s="41" t="s"/>
       <c r="C68" s="42" t="s"/>
       <c r="D68" s="43" t="s"/>
-      <c r="E68" s="69" t="s"/>
+      <c r="E68" s="62" t="s"/>
       <c r="F68" s="42" t="s"/>
       <c r="G68" s="42" t="s"/>
       <c r="H68" s="42" t="s"/>
@@ -3663,13 +3683,14 @@
       <c r="L68" s="44" t="s"/>
       <c r="M68" s="44" t="s"/>
       <c r="N68" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="69" s="32" spans="1:14">
+      <c r="O68" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="69" s="32" spans="1:15">
       <c r="A69" s="40" t="s"/>
       <c r="B69" s="41" t="s"/>
       <c r="C69" s="42" t="s"/>
       <c r="D69" s="43" t="s"/>
-      <c r="E69" s="69" t="s"/>
+      <c r="E69" s="62" t="s"/>
       <c r="F69" s="40" t="s"/>
       <c r="G69" s="40" t="s"/>
       <c r="H69" s="40" t="s"/>
@@ -3679,13 +3700,14 @@
       <c r="L69" s="44" t="s"/>
       <c r="M69" s="44" t="s"/>
       <c r="N69" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="70" s="32" spans="1:14">
+      <c r="O69" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="70" s="32" spans="1:15">
       <c r="A70" s="40" t="s"/>
       <c r="B70" s="41" t="s"/>
       <c r="C70" s="42" t="s"/>
       <c r="D70" s="43" t="s"/>
-      <c r="E70" s="69" t="s"/>
+      <c r="E70" s="62" t="s"/>
       <c r="F70" s="42" t="s"/>
       <c r="G70" s="42" t="s"/>
       <c r="H70" s="42" t="s"/>
@@ -3695,13 +3717,14 @@
       <c r="L70" s="44" t="s"/>
       <c r="M70" s="44" t="s"/>
       <c r="N70" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="71" s="32" spans="1:14">
+      <c r="O70" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="71" s="32" spans="1:15">
       <c r="A71" s="40" t="s"/>
       <c r="B71" s="41" t="s"/>
       <c r="C71" s="42" t="s"/>
       <c r="D71" s="43" t="s"/>
-      <c r="E71" s="69" t="s"/>
+      <c r="E71" s="62" t="s"/>
       <c r="F71" s="40" t="s"/>
       <c r="G71" s="40" t="s"/>
       <c r="H71" s="40" t="s"/>
@@ -3711,13 +3734,14 @@
       <c r="L71" s="44" t="s"/>
       <c r="M71" s="44" t="s"/>
       <c r="N71" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="72" s="32" spans="1:14">
+      <c r="O71" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="72" s="32" spans="1:15">
       <c r="A72" s="40" t="s"/>
       <c r="B72" s="41" t="s"/>
       <c r="C72" s="42" t="s"/>
       <c r="D72" s="43" t="s"/>
-      <c r="E72" s="69" t="s"/>
+      <c r="E72" s="62" t="s"/>
       <c r="F72" s="42" t="s"/>
       <c r="G72" s="42" t="s"/>
       <c r="H72" s="42" t="s"/>
@@ -3727,13 +3751,14 @@
       <c r="L72" s="44" t="s"/>
       <c r="M72" s="44" t="s"/>
       <c r="N72" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="73" s="32" spans="1:14">
+      <c r="O72" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="73" s="32" spans="1:15">
       <c r="A73" s="40" t="s"/>
       <c r="B73" s="41" t="s"/>
       <c r="C73" s="42" t="s"/>
       <c r="D73" s="43" t="s"/>
-      <c r="E73" s="69" t="s"/>
+      <c r="E73" s="62" t="s"/>
       <c r="F73" s="40" t="s"/>
       <c r="G73" s="40" t="s"/>
       <c r="H73" s="40" t="s"/>
@@ -3743,13 +3768,14 @@
       <c r="L73" s="44" t="s"/>
       <c r="M73" s="44" t="s"/>
       <c r="N73" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="74" s="32" spans="1:14">
+      <c r="O73" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="74" s="32" spans="1:15">
       <c r="A74" s="40" t="s"/>
       <c r="B74" s="41" t="s"/>
       <c r="C74" s="42" t="s"/>
       <c r="D74" s="43" t="s"/>
-      <c r="E74" s="69" t="s"/>
+      <c r="E74" s="62" t="s"/>
       <c r="F74" s="42" t="s"/>
       <c r="G74" s="42" t="s"/>
       <c r="H74" s="42" t="s"/>
@@ -3759,13 +3785,14 @@
       <c r="L74" s="44" t="s"/>
       <c r="M74" s="44" t="s"/>
       <c r="N74" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="75" s="32" spans="1:14">
+      <c r="O74" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="75" s="32" spans="1:15">
       <c r="A75" s="40" t="s"/>
       <c r="B75" s="41" t="s"/>
       <c r="C75" s="42" t="s"/>
       <c r="D75" s="43" t="s"/>
-      <c r="E75" s="69" t="s"/>
+      <c r="E75" s="62" t="s"/>
       <c r="F75" s="40" t="s"/>
       <c r="G75" s="40" t="s"/>
       <c r="H75" s="40" t="s"/>
@@ -3775,8 +3802,9 @@
       <c r="L75" s="44" t="s"/>
       <c r="M75" s="44" t="s"/>
       <c r="N75" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="76" s="32" spans="1:14">
+      <c r="O75" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="76" s="32" spans="1:15">
       <c r="A76" s="40" t="s"/>
       <c r="B76" s="41" t="s"/>
       <c r="C76" s="42" t="s"/>
@@ -3791,8 +3819,9 @@
       <c r="L76" s="44" t="s"/>
       <c r="M76" s="44" t="s"/>
       <c r="N76" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="77" s="32" spans="1:14">
+      <c r="O76" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="77" s="32" spans="1:15">
       <c r="A77" s="40" t="s"/>
       <c r="B77" s="41" t="s"/>
       <c r="C77" s="42" t="s"/>
@@ -3807,8 +3836,9 @@
       <c r="L77" s="44" t="s"/>
       <c r="M77" s="44" t="s"/>
       <c r="N77" s="45" t="s"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="78" s="32" spans="1:14">
+      <c r="O77" t="s"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="78" s="32" spans="1:15">
       <c r="A78" s="40" t="s"/>
       <c r="B78" s="41" t="s"/>
       <c r="C78" s="42" t="s"/>
@@ -3823,8 +3853,9 @@
       <c r="L78" s="44" t="s"/>
       <c r="M78" s="44" t="s"/>
       <c r="N78" s="45" t="s"/>
-    </row>
-    <row r="79" spans="1:14">
+      <c r="O78" t="s"/>
+    </row>
+    <row r="79" spans="1:15">
       <c r="A79" s="39" t="s"/>
       <c r="B79" t="s"/>
       <c r="C79" t="s"/>
@@ -3839,6 +3870,7 @@
       <c r="L79" t="s"/>
       <c r="M79" t="s"/>
       <c r="N79" t="s"/>
+      <c r="O79" t="s"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -3878,41 +3910,41 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="I2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="J2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="K2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="M2" t="s">
         <v>1</v>
       </c>
       <c r="O2" s="53" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="Q2" s="22" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="R2" s="53" t="n"/>
       <c r="T2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="W2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="Y2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="Z2" s="53" t="s">
         <v>3</v>
@@ -4028,7 +4060,7 @@
         <v/>
       </c>
       <c r="Q4" s="54" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="R4" s="53" t="n">
         <v>1</v>
@@ -4088,7 +4120,7 @@
         <v/>
       </c>
       <c r="Q5" s="54" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="R5" s="53" t="n">
         <v>2</v>
@@ -4148,7 +4180,7 @@
         <v/>
       </c>
       <c r="Q6" s="54" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R6" s="53" t="n">
         <v>3</v>
@@ -4208,7 +4240,7 @@
         <v/>
       </c>
       <c r="Q7" s="54" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="R7" s="53" t="n">
         <v>4</v>
@@ -4256,7 +4288,7 @@
         <v/>
       </c>
       <c r="Q8" s="54" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="R8" s="53" t="n">
         <v>5</v>
@@ -4300,7 +4332,7 @@
         <v>6</v>
       </c>
       <c r="Q9" s="54" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="R9" s="53" t="n">
         <v>6</v>
@@ -4338,10 +4370,10 @@
         <v>7</v>
       </c>
       <c r="I10" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="Q10" s="54" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="R10" s="53" t="n">
         <v>7</v>
@@ -4381,7 +4413,7 @@
         <v/>
       </c>
       <c r="Q11" s="54" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="R11" s="53" t="n">
         <v>8</v>
@@ -4417,7 +4449,7 @@
         <v>9</v>
       </c>
       <c r="Q12" s="54" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="R12" s="53" t="n">
         <v>9</v>
@@ -4450,10 +4482,10 @@
         <v>10</v>
       </c>
       <c r="G13" s="53" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="Q13" s="53" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="R13" s="53" t="n">
         <v>10</v>
@@ -4486,10 +4518,10 @@
         <v>11</v>
       </c>
       <c r="G14" s="53" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="Q14" s="53" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="R14" s="53" t="n">
         <v>11</v>
@@ -4522,10 +4554,10 @@
         <v>12</v>
       </c>
       <c r="G15" s="53" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="Q15" s="53" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="R15" s="53" t="n">
         <v>12</v>
@@ -4558,10 +4590,10 @@
         <v>13</v>
       </c>
       <c r="G16" s="53" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="Q16" s="53" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="R16" s="53" t="n">
         <v>13</v>
@@ -4594,10 +4626,10 @@
         <v>14</v>
       </c>
       <c r="G17" s="53" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="Q17" s="53" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="R17" s="53" t="n">
         <v>14</v>
@@ -4630,10 +4662,10 @@
         <v>15</v>
       </c>
       <c r="G18" s="53" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="Q18" s="53" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="R18" s="53" t="n">
         <v>15</v>
@@ -4666,10 +4698,10 @@
         <v>16</v>
       </c>
       <c r="G19" s="53" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="Q19" s="53" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="R19" s="53" t="n">
         <v>16</v>
@@ -4702,10 +4734,10 @@
         <v>17</v>
       </c>
       <c r="G20" s="53" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="Q20" s="53" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="R20" s="53" t="n">
         <v>17</v>
@@ -4738,10 +4770,10 @@
         <v>18</v>
       </c>
       <c r="G21" s="53" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="Q21" s="53" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="R21" s="53" t="n">
         <v>18</v>
@@ -4774,10 +4806,10 @@
         <v>19</v>
       </c>
       <c r="G22" s="53" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="Q22" s="53" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="R22" s="53" t="n">
         <v>19</v>
@@ -4810,10 +4842,10 @@
         <v>20</v>
       </c>
       <c r="G23" s="53" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="Q23" s="53" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="R23" s="53" t="n">
         <v>20</v>
@@ -4846,10 +4878,10 @@
         <v>21</v>
       </c>
       <c r="G24" s="53" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="Q24" s="53" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="R24" s="53" t="n">
         <v>21</v>
@@ -4882,10 +4914,10 @@
         <v>22</v>
       </c>
       <c r="G25" s="53" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="Q25" s="53" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="R25" s="53" t="n">
         <v>22</v>
@@ -4918,10 +4950,10 @@
         <v>23</v>
       </c>
       <c r="G26" s="53" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="Q26" s="53" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="R26" s="53" t="n">
         <v>23</v>
@@ -4943,10 +4975,10 @@
         <v>24</v>
       </c>
       <c r="G27" s="53" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="Q27" s="53" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="R27" s="53" t="n">
         <v>24</v>
@@ -4957,10 +4989,10 @@
         <v>25</v>
       </c>
       <c r="G28" s="53" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="Q28" s="53" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="R28" s="53" t="n">
         <v>25</v>
@@ -4971,10 +5003,10 @@
         <v>26</v>
       </c>
       <c r="G29" s="53" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="Q29" s="53" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="R29" s="53" t="n">
         <v>26</v>
@@ -4985,10 +5017,10 @@
         <v>27</v>
       </c>
       <c r="G30" s="53" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="Q30" s="53" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="R30" s="53" t="n">
         <v>27</v>
@@ -4999,10 +5031,10 @@
         <v>28</v>
       </c>
       <c r="G31" s="53" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="Q31" s="53" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="R31" s="53" t="n">
         <v>28</v>
@@ -5013,10 +5045,10 @@
         <v>29</v>
       </c>
       <c r="G32" s="53" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="Q32" s="53" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="R32" s="53" t="n">
         <v>29</v>
@@ -5080,13 +5112,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -5094,10 +5126,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C2" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -5105,10 +5137,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C3" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -5116,10 +5148,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C4" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -5127,10 +5159,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C5" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -5138,10 +5170,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C6" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -5149,10 +5181,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C7" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -5160,10 +5192,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C8" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -5171,10 +5203,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C9" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -5182,10 +5214,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C10" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -5193,10 +5225,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C11" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -5204,10 +5236,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C12" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -5215,10 +5247,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C13" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -5226,10 +5258,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C14" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -5237,10 +5269,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C15" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -5248,10 +5280,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C16" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -5259,10 +5291,10 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C17" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -5270,10 +5302,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C18" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -5281,10 +5313,10 @@
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C19" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -5292,10 +5324,10 @@
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C20" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -5303,10 +5335,10 @@
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C21" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -5314,10 +5346,10 @@
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C22" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -5325,10 +5357,10 @@
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C23" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -5336,10 +5368,10 @@
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C24" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -5347,35 +5379,35 @@
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C25" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="B26" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="B27" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="B28" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="B29" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="B30" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>